<commit_message>
Actualizacion de Cronograma y Desempeño
</commit_message>
<xml_diff>
--- a/P3GA1/Prototipo_2P-master/Cronograma GA1.xlsx
+++ b/P3GA1/Prototipo_2P-master/Cronograma GA1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SEBAS\Desktop\P\P3GA1\Prototipo_2P-master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{86296A00-1B96-4D28-8CBF-713DE6C590E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{847A817C-C30C-4F5C-94CD-55007DC28FD9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="31">
   <si>
     <t>N°</t>
   </si>
@@ -111,6 +111,21 @@
   </si>
   <si>
     <t>Verificación del funcionamiento</t>
+  </si>
+  <si>
+    <t>Creacion form Registro Usuarios</t>
+  </si>
+  <si>
+    <t>Cambio de diseño de Registro usuarios</t>
+  </si>
+  <si>
+    <t>Creacion form Login</t>
+  </si>
+  <si>
+    <t>Cambio de diseño de Login</t>
+  </si>
+  <si>
+    <t>Creacion de tabla usuarios</t>
   </si>
 </sst>
 </file>
@@ -172,15 +187,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
@@ -464,10 +477,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:H21"/>
+  <dimension ref="B2:H28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -501,147 +514,147 @@
       </c>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B3" s="5">
-        <v>1</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="5" t="s">
+      <c r="B3" s="4">
+        <v>1</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="6">
-        <v>43963</v>
-      </c>
-      <c r="F3" s="7">
-        <v>0</v>
-      </c>
-      <c r="G3" s="6">
+      <c r="E3" s="5">
+        <v>43963</v>
+      </c>
+      <c r="F3" s="4">
+        <v>0</v>
+      </c>
+      <c r="G3" s="5">
         <f>+E3+F3</f>
         <v>43963</v>
       </c>
-      <c r="H3" s="8">
+      <c r="H3" s="6">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="5">
+      <c r="B4" s="4">
         <v>2</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="6">
-        <v>43963</v>
-      </c>
-      <c r="F4" s="7">
-        <v>0</v>
-      </c>
-      <c r="G4" s="6">
-        <f t="shared" ref="G4:G16" si="0">+E4+F4</f>
-        <v>43963</v>
-      </c>
-      <c r="H4" s="8">
+      <c r="E4" s="5">
+        <v>43963</v>
+      </c>
+      <c r="F4" s="4">
+        <v>0</v>
+      </c>
+      <c r="G4" s="5">
+        <f t="shared" ref="G4:G23" si="0">+E4+F4</f>
+        <v>43963</v>
+      </c>
+      <c r="H4" s="6">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B5" s="5">
+      <c r="B5" s="4">
         <v>3</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="6">
-        <v>43963</v>
-      </c>
-      <c r="F5" s="7">
-        <v>0</v>
-      </c>
-      <c r="G5" s="6">
-        <f t="shared" si="0"/>
-        <v>43963</v>
-      </c>
-      <c r="H5" s="8">
+      <c r="E5" s="5">
+        <v>43963</v>
+      </c>
+      <c r="F5" s="4">
+        <v>0</v>
+      </c>
+      <c r="G5" s="5">
+        <f t="shared" si="0"/>
+        <v>43963</v>
+      </c>
+      <c r="H5" s="6">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B6" s="5">
+      <c r="B6" s="4">
         <v>4</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="6">
-        <v>43963</v>
-      </c>
-      <c r="F6" s="7">
-        <v>0</v>
-      </c>
-      <c r="G6" s="6">
-        <f t="shared" si="0"/>
-        <v>43963</v>
-      </c>
-      <c r="H6" s="8">
+      <c r="E6" s="5">
+        <v>43963</v>
+      </c>
+      <c r="F6" s="4">
+        <v>0</v>
+      </c>
+      <c r="G6" s="5">
+        <f t="shared" si="0"/>
+        <v>43963</v>
+      </c>
+      <c r="H6" s="6">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="5">
+      <c r="B7" s="4">
         <v>5</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E7" s="6">
-        <v>43963</v>
-      </c>
-      <c r="F7" s="7">
-        <v>0</v>
-      </c>
-      <c r="G7" s="6">
-        <f t="shared" si="0"/>
-        <v>43963</v>
-      </c>
-      <c r="H7" s="8">
-        <v>0</v>
+      <c r="E7" s="5">
+        <v>43963</v>
+      </c>
+      <c r="F7" s="4">
+        <v>0</v>
+      </c>
+      <c r="G7" s="5">
+        <f t="shared" si="0"/>
+        <v>43963</v>
+      </c>
+      <c r="H7" s="6">
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B8" s="5">
+      <c r="B8" s="4">
         <v>6</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E8" s="6">
-        <v>43963</v>
-      </c>
-      <c r="F8" s="7">
-        <v>1</v>
-      </c>
-      <c r="G8" s="6">
+      <c r="E8" s="5">
+        <v>43963</v>
+      </c>
+      <c r="F8" s="4">
+        <v>1</v>
+      </c>
+      <c r="G8" s="5">
         <f t="shared" si="0"/>
         <v>43964</v>
       </c>
-      <c r="H8" s="8">
-        <v>0</v>
+      <c r="H8" s="6">
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
@@ -652,68 +665,68 @@
         <v>7</v>
       </c>
       <c r="D9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="2">
+        <v>43963</v>
+      </c>
+      <c r="F9" s="1">
+        <v>1</v>
+      </c>
+      <c r="G9" s="2">
+        <f t="shared" si="0"/>
+        <v>43964</v>
+      </c>
+      <c r="H9" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B10" s="4">
+        <v>8</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" s="5">
+        <v>43963</v>
+      </c>
+      <c r="F10" s="4">
+        <v>1</v>
+      </c>
+      <c r="G10" s="5">
+        <f t="shared" si="0"/>
+        <v>43964</v>
+      </c>
+      <c r="H10" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B11" s="4">
+        <v>9</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="2">
-        <v>43963</v>
-      </c>
-      <c r="F9" s="3">
-        <v>1</v>
-      </c>
-      <c r="G9" s="2">
-        <f t="shared" si="0"/>
+      <c r="E11" s="5">
         <v>43964</v>
       </c>
-      <c r="H9" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="5">
-        <v>8</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="E10" s="6">
-        <v>43963</v>
-      </c>
-      <c r="F10" s="7">
-        <v>2</v>
-      </c>
-      <c r="G10" s="6">
-        <f t="shared" si="0"/>
-        <v>43965</v>
-      </c>
-      <c r="H10" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="5">
-        <v>9</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E11" s="6">
-        <v>43965</v>
-      </c>
-      <c r="F11" s="7">
-        <v>0</v>
-      </c>
-      <c r="G11" s="6">
-        <f t="shared" si="0"/>
-        <v>43965</v>
-      </c>
-      <c r="H11" s="8">
-        <v>0</v>
+      <c r="F11" s="4">
+        <v>0</v>
+      </c>
+      <c r="G11" s="5">
+        <f t="shared" si="0"/>
+        <v>43964</v>
+      </c>
+      <c r="H11" s="6">
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
@@ -729,86 +742,86 @@
       <c r="E12" s="2">
         <v>43963</v>
       </c>
-      <c r="F12" s="3">
-        <v>1</v>
+      <c r="F12" s="1">
+        <v>0</v>
       </c>
       <c r="G12" s="2">
         <f t="shared" si="0"/>
+        <v>43963</v>
+      </c>
+      <c r="H12" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B13" s="4">
+        <v>11</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E13" s="5">
+        <v>43963</v>
+      </c>
+      <c r="F13" s="4">
+        <v>2</v>
+      </c>
+      <c r="G13" s="5">
+        <f t="shared" si="0"/>
+        <v>43965</v>
+      </c>
+      <c r="H13" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B14" s="4">
+        <v>12</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E14" s="5">
         <v>43964</v>
       </c>
-      <c r="H12" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B13" s="5">
-        <v>11</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="E13" s="6">
-        <v>43963</v>
-      </c>
-      <c r="F13" s="7">
-        <v>2</v>
-      </c>
-      <c r="G13" s="6">
-        <f t="shared" si="0"/>
+      <c r="F14" s="4">
+        <v>0</v>
+      </c>
+      <c r="G14" s="5">
+        <f t="shared" si="0"/>
+        <v>43964</v>
+      </c>
+      <c r="H14" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B15" s="1">
+        <v>13</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" s="2">
         <v>43965</v>
       </c>
-      <c r="H13" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B14" s="5">
-        <v>12</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E14" s="6">
+      <c r="F15" s="1">
+        <v>0</v>
+      </c>
+      <c r="G15" s="2">
+        <f t="shared" si="0"/>
         <v>43965</v>
       </c>
-      <c r="F14" s="7">
-        <v>0</v>
-      </c>
-      <c r="G14" s="6">
-        <f t="shared" si="0"/>
-        <v>43965</v>
-      </c>
-      <c r="H14" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B15" s="5">
-        <v>13</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E15" s="6">
-        <v>43963</v>
-      </c>
-      <c r="F15" s="7">
-        <v>2</v>
-      </c>
-      <c r="G15" s="6">
-        <f t="shared" si="0"/>
-        <v>43965</v>
-      </c>
-      <c r="H15" s="8">
+      <c r="H15" s="3">
         <v>0</v>
       </c>
     </row>
@@ -817,46 +830,214 @@
         <v>14</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E16" s="2">
+        <v>43963</v>
+      </c>
+      <c r="F16" s="1">
+        <v>0</v>
+      </c>
+      <c r="G16" s="2">
+        <f t="shared" si="0"/>
+        <v>43963</v>
+      </c>
+      <c r="H16" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B17" s="4">
+        <v>15</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E17" s="5">
+        <v>43963</v>
+      </c>
+      <c r="F17" s="4">
+        <v>0</v>
+      </c>
+      <c r="G17" s="5">
+        <f t="shared" si="0"/>
+        <v>43963</v>
+      </c>
+      <c r="H17" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B18" s="4">
+        <v>16</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E18" s="5">
+        <v>43963</v>
+      </c>
+      <c r="F18" s="4">
+        <v>1</v>
+      </c>
+      <c r="G18" s="5">
+        <f t="shared" si="0"/>
+        <v>43964</v>
+      </c>
+      <c r="H18" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B19" s="1">
+        <v>17</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E19" s="2">
+        <v>43963</v>
+      </c>
+      <c r="F19" s="1">
+        <v>0</v>
+      </c>
+      <c r="G19" s="2">
+        <f t="shared" si="0"/>
+        <v>43963</v>
+      </c>
+      <c r="H19" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B20" s="4">
+        <v>18</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E20" s="5">
+        <v>43963</v>
+      </c>
+      <c r="F20" s="4">
+        <v>0</v>
+      </c>
+      <c r="G20" s="5">
+        <f t="shared" si="0"/>
+        <v>43963</v>
+      </c>
+      <c r="H20" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B21" s="4">
+        <v>19</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E21" s="5">
+        <v>43963</v>
+      </c>
+      <c r="F21" s="4">
+        <v>1</v>
+      </c>
+      <c r="G21" s="5">
+        <f t="shared" si="0"/>
+        <v>43964</v>
+      </c>
+      <c r="H21" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B22" s="4">
+        <v>20</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E22" s="5">
+        <v>43963</v>
+      </c>
+      <c r="F22" s="4">
+        <v>0</v>
+      </c>
+      <c r="G22" s="5">
+        <f t="shared" si="0"/>
+        <v>43963</v>
+      </c>
+      <c r="H22" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B23" s="4">
+        <v>21</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E23" s="5">
+        <v>43963</v>
+      </c>
+      <c r="F23" s="4">
+        <v>2</v>
+      </c>
+      <c r="G23" s="5">
+        <f t="shared" si="0"/>
         <v>43965</v>
       </c>
-      <c r="F16" s="3">
-        <v>0</v>
-      </c>
-      <c r="G16" s="2">
-        <f t="shared" si="0"/>
-        <v>43965</v>
-      </c>
-      <c r="H16" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="H17" s="9">
-        <f>AVERAGE(H3:H16)</f>
-        <v>0.2857142857142857</v>
-      </c>
-    </row>
-    <row r="20" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D20" s="1" t="s">
+      <c r="H23" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H24" s="7">
+        <f>AVERAGE(H3:H23)</f>
+        <v>0.8571428571428571</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D27" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E20" s="6">
+      <c r="E27" s="5">
         <f>+E3</f>
         <v>43963</v>
       </c>
     </row>
-    <row r="21" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D21" s="1" t="s">
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D28" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E21" s="6">
-        <f>+G16</f>
+      <c r="E28" s="5">
+        <f>+G15</f>
         <v>43965</v>
       </c>
     </row>

</xml_diff>